<commit_message>
Ajuste Formato fecha de yyyy/mm/dd a formato dd/mm/yyyy
</commit_message>
<xml_diff>
--- a/blocks/inventarios/asignarInventarioC/gestionContratistas/plantilla/archivo_contratista.xlsx
+++ b/blocks/inventarios/asignarInventarioC/gestionContratistas/plantilla/archivo_contratista.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>Tipo de Contrato</t>
   </si>
@@ -39,40 +39,28 @@
     <t>MICHAEL STIV VERDUGO</t>
   </si>
   <si>
-    <t>2015/10/15</t>
-  </si>
-  <si>
-    <t>2016/10/12</t>
-  </si>
-  <si>
-    <t>2015/10/16</t>
-  </si>
-  <si>
-    <t>2016/10/13</t>
+    <t>01/01/2016</t>
+  </si>
+  <si>
+    <t>12/12/2016</t>
+  </si>
+  <si>
+    <t>12/12/2017</t>
   </si>
   <si>
     <t>VIOLETA   ANA LUZ SOSA</t>
   </si>
   <si>
-    <t>2015/10/17</t>
-  </si>
-  <si>
-    <t>2016/10/14</t>
-  </si>
-  <si>
-    <t>2015/10/18</t>
-  </si>
-  <si>
-    <t>2016/10/15</t>
+    <t>12/12/2018</t>
+  </si>
+  <si>
+    <t>12/12/2019</t>
   </si>
   <si>
     <t>DIANA LEONOR TINJACA</t>
   </si>
   <si>
-    <t>2015/10/19</t>
-  </si>
-  <si>
-    <t>2016/10/16</t>
+    <t>12/12/2020</t>
   </si>
   <si>
     <t>TIPO DE CONTRATO</t>
@@ -84,7 +72,7 @@
     <t>FORMATO DE FECHA</t>
   </si>
   <si>
-    <t>El formato de fecha es Año Mes Día delimitados por  “/ ”</t>
+    <t>El formato de fecha es Año Mes Día delimitados por  “/ ” , dia/mes/año por ejemplo : 01/10/2016</t>
   </si>
   <si>
     <t>2  : Contrato de Prestación Servicios</t>
@@ -94,8 +82,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -197,19 +186,31 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -222,7 +223,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -246,7 +251,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="E:F"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -255,8 +260,8 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.6326530612245"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.6836734693878"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.2244897959184"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.1020408163265"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.1530612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.1020408163265"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="42.1530612244898"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="34.7755102040816"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="42.1530612244898"/>
     <col collapsed="false" hidden="false" max="10" min="9" style="0" width="32.3724489795918"/>
@@ -269,22 +274,22 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -293,8 +298,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -306,8 +311,8 @@
   </sheetPr>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="E:F"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -316,35 +321,35 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.6734693877551"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.030612244898"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.1785714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.9540816326531"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.7295918367347"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="26.9540816326531"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="37.3724489795918"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.8316326530612"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="0" width="22.2551020408163"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="n">
+      <c r="A2" s="6" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="n">
@@ -356,15 +361,15 @@
       <c r="D2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
+      <c r="A3" s="6" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -376,15 +381,15 @@
       <c r="D3" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="n">
+      <c r="A4" s="6" t="n">
         <v>1</v>
       </c>
       <c r="B4" s="0" t="n">
@@ -394,17 +399,17 @@
         <v>1237651763</v>
       </c>
       <c r="D4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="n">
+      <c r="A5" s="6" t="n">
         <v>2</v>
       </c>
       <c r="B5" s="0" t="n">
@@ -414,17 +419,17 @@
         <v>1237651763</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>15</v>
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="n">
+      <c r="A6" s="6" t="n">
         <v>2</v>
       </c>
       <c r="B6" s="0" t="n">
@@ -434,42 +439,42 @@
         <v>5535353533</v>
       </c>
       <c r="D6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F8" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="10"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="6"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -483,8 +488,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>